<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@68e9728a677488929d90bce78458c2456a05ac65 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-location.xlsx
+++ b/StructureDefinition-us-core-location.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="331">
   <si>
     <t>Property</t>
   </si>
@@ -146,6 +146,10 @@
   </si>
   <si>
     <t>\-</t>
+  </si>
+  <si>
+    <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
   <si>
     <t>.Role[classCode=SDLC]</t>
@@ -1513,10 +1517,10 @@
         <v>37</v>
       </c>
       <c r="AJ1" t="s" s="2">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="AK1" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AL1" t="s" s="2">
         <v>37</v>
@@ -1524,10 +1528,10 @@
     </row>
     <row r="2" hidden="true">
       <c r="A2" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s" s="2">
@@ -1538,7 +1542,7 @@
         <v>38</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s" s="2">
         <v>37</v>
@@ -1547,19 +1551,19 @@
         <v>37</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M2" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N2" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O2" s="2"/>
       <c r="P2" t="s" s="2">
@@ -1609,13 +1613,13 @@
         <v>37</v>
       </c>
       <c r="AF2" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AG2" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI2" t="s" s="2">
         <v>37</v>
@@ -1632,10 +1636,10 @@
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
@@ -1646,7 +1650,7 @@
         <v>38</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s" s="2">
         <v>37</v>
@@ -1655,16 +1659,16 @@
         <v>37</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1715,19 +1719,19 @@
         <v>37</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AG3" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI3" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK3" t="s" s="2">
         <v>37</v>
@@ -1738,10 +1742,10 @@
     </row>
     <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
@@ -1752,28 +1756,28 @@
         <v>38</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H4" t="s" s="2">
         <v>37</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N4" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" t="s" s="2">
@@ -1823,19 +1827,19 @@
         <v>37</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AG4" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI4" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK4" t="s" s="2">
         <v>37</v>
@@ -1846,10 +1850,10 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
@@ -1860,7 +1864,7 @@
         <v>38</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>37</v>
@@ -1872,16 +1876,16 @@
         <v>37</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N5" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
@@ -1907,13 +1911,13 @@
         <v>37</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y5" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Z5" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AA5" t="s" s="2">
         <v>37</v>
@@ -1931,19 +1935,19 @@
         <v>37</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI5" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK5" t="s" s="2">
         <v>37</v>
@@ -1954,21 +1958,21 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s" s="2">
         <v>37</v>
@@ -1980,16 +1984,16 @@
         <v>37</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N6" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
@@ -2039,22 +2043,22 @@
         <v>37</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AG6" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI6" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AL6" t="s" s="2">
         <v>37</v>
@@ -2062,14 +2066,14 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
@@ -2088,16 +2092,16 @@
         <v>37</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N7" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" t="s" s="2">
@@ -2147,7 +2151,7 @@
         <v>37</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>38</v>
@@ -2162,7 +2166,7 @@
         <v>37</v>
       </c>
       <c r="AK7" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AL7" t="s" s="2">
         <v>37</v>
@@ -2170,14 +2174,14 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
@@ -2196,16 +2200,16 @@
         <v>37</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N8" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" t="s" s="2">
@@ -2255,7 +2259,7 @@
         <v>37</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AG8" t="s" s="2">
         <v>38</v>
@@ -2267,10 +2271,10 @@
         <v>37</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AK8" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AL8" t="s" s="2">
         <v>37</v>
@@ -2278,14 +2282,14 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="2">
@@ -2298,25 +2302,25 @@
         <v>37</v>
       </c>
       <c r="I9" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J9" t="s" s="2">
         <v>37</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N9" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O9" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="P9" t="s" s="2">
         <v>37</v>
@@ -2365,7 +2369,7 @@
         <v>37</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AG9" t="s" s="2">
         <v>38</v>
@@ -2377,10 +2381,10 @@
         <v>37</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AL9" t="s" s="2">
         <v>37</v>
@@ -2388,10 +2392,10 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
@@ -2405,26 +2409,26 @@
         <v>39</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I10" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="P10" t="s" s="2">
         <v>37</v>
@@ -2473,7 +2477,7 @@
         <v>37</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>38</v>
@@ -2485,21 +2489,21 @@
         <v>37</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AL10" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
@@ -2510,25 +2514,25 @@
         <v>38</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -2555,13 +2559,13 @@
         <v>37</v>
       </c>
       <c r="X11" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Y11" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Z11" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AA11" t="s" s="2">
         <v>37</v>
@@ -2579,33 +2583,33 @@
         <v>37</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI11" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -2616,7 +2620,7 @@
         <v>38</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H12" t="s" s="2">
         <v>37</v>
@@ -2625,16 +2629,16 @@
         <v>37</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -2661,13 +2665,13 @@
         <v>37</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Z12" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AA12" t="s" s="2">
         <v>37</v>
@@ -2685,33 +2689,33 @@
         <v>37</v>
       </c>
       <c r="AF12" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="AG12" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH12" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AI12" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AJ12" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="AK12" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="AL12" t="s" s="2">
         <v>117</v>
-      </c>
-      <c r="AG12" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AH12" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AJ12" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="AK12" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="AL12" t="s" s="2">
-        <v>116</v>
       </c>
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -2719,31 +2723,31 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I13" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" t="s" s="2">
@@ -2793,22 +2797,22 @@
         <v>37</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI13" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AL13" t="s" s="2">
         <v>37</v>
@@ -2816,10 +2820,10 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -2842,19 +2846,19 @@
         <v>37</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N14" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="O14" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="P14" t="s" s="2">
         <v>37</v>
@@ -2903,7 +2907,7 @@
         <v>37</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>38</v>
@@ -2915,10 +2919,10 @@
         <v>37</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>37</v>
@@ -2926,10 +2930,10 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -2940,7 +2944,7 @@
         <v>38</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>37</v>
@@ -2949,20 +2953,20 @@
         <v>37</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="P15" t="s" s="2">
         <v>37</v>
@@ -3011,22 +3015,22 @@
         <v>37</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI15" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AL15" t="s" s="2">
         <v>37</v>
@@ -3034,10 +3038,10 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -3048,7 +3052,7 @@
         <v>38</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>37</v>
@@ -3057,22 +3061,22 @@
         <v>37</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="O16" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="P16" t="s" s="2">
         <v>37</v>
@@ -3097,13 +3101,13 @@
         <v>37</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="Z16" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AA16" t="s" s="2">
         <v>37</v>
@@ -3121,33 +3125,33 @@
         <v>37</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH16" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI16" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -3161,22 +3165,22 @@
         <v>39</v>
       </c>
       <c r="H17" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I17" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -3203,11 +3207,11 @@
         <v>37</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="Y17" s="2"/>
       <c r="Z17" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AA17" t="s" s="2">
         <v>37</v>
@@ -3225,7 +3229,7 @@
         <v>37</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>38</v>
@@ -3237,21 +3241,21 @@
         <v>37</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3265,7 +3269,7 @@
         <v>39</v>
       </c>
       <c r="H18" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I18" t="s" s="2">
         <v>37</v>
@@ -3274,13 +3278,13 @@
         <v>37</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -3331,7 +3335,7 @@
         <v>37</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>38</v>
@@ -3343,10 +3347,10 @@
         <v>37</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AL18" t="s" s="2">
         <v>37</v>
@@ -3354,10 +3358,10 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3368,10 +3372,10 @@
         <v>38</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I19" t="s" s="2">
         <v>37</v>
@@ -3380,19 +3384,19 @@
         <v>37</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="O19" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="P19" t="s" s="2">
         <v>37</v>
@@ -3441,22 +3445,22 @@
         <v>37</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI19" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>37</v>
@@ -3464,10 +3468,10 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3478,7 +3482,7 @@
         <v>38</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>37</v>
@@ -3490,13 +3494,13 @@
         <v>37</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -3547,13 +3551,13 @@
         <v>37</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH20" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI20" t="s" s="2">
         <v>37</v>
@@ -3562,7 +3566,7 @@
         <v>37</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>37</v>
@@ -3570,14 +3574,14 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" t="s" s="2">
@@ -3596,16 +3600,16 @@
         <v>37</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" t="s" s="2">
@@ -3643,19 +3647,19 @@
         <v>37</v>
       </c>
       <c r="AB21" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AC21" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AD21" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>38</v>
@@ -3667,10 +3671,10 @@
         <v>37</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>37</v>
@@ -3678,10 +3682,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -3692,31 +3696,31 @@
         <v>38</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>37</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="O22" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="P22" t="s" s="2">
         <v>37</v>
@@ -3729,7 +3733,7 @@
         <v>37</v>
       </c>
       <c r="T22" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U22" t="s" s="2">
         <v>37</v>
@@ -3741,13 +3745,13 @@
         <v>37</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Z22" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AA22" t="s" s="2">
         <v>37</v>
@@ -3765,22 +3769,22 @@
         <v>37</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>37</v>
@@ -3788,10 +3792,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -3802,7 +3806,7 @@
         <v>38</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>37</v>
@@ -3811,19 +3815,19 @@
         <v>37</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" t="s" s="2">
@@ -3837,7 +3841,7 @@
         <v>37</v>
       </c>
       <c r="T23" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="U23" t="s" s="2">
         <v>37</v>
@@ -3849,13 +3853,13 @@
         <v>37</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="Z23" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AA23" t="s" s="2">
         <v>37</v>
@@ -3873,22 +3877,22 @@
         <v>37</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>37</v>
@@ -3896,10 +3900,10 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -3910,7 +3914,7 @@
         <v>38</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H24" t="s" s="2">
         <v>37</v>
@@ -3919,22 +3923,22 @@
         <v>37</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="O24" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="P24" t="s" s="2">
         <v>37</v>
@@ -3947,7 +3951,7 @@
         <v>37</v>
       </c>
       <c r="T24" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U24" t="s" s="2">
         <v>37</v>
@@ -3983,22 +3987,22 @@
         <v>37</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>37</v>
@@ -4006,10 +4010,10 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4023,22 +4027,22 @@
         <v>39</v>
       </c>
       <c r="H25" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I25" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -4053,7 +4057,7 @@
         <v>37</v>
       </c>
       <c r="T25" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="U25" t="s" s="2">
         <v>37</v>
@@ -4089,7 +4093,7 @@
         <v>37</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>38</v>
@@ -4101,10 +4105,10 @@
         <v>37</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>37</v>
@@ -4112,39 +4116,39 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H26" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I26" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -4159,7 +4163,7 @@
         <v>37</v>
       </c>
       <c r="T26" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="U26" t="s" s="2">
         <v>37</v>
@@ -4195,22 +4199,22 @@
         <v>37</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI26" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>37</v>
@@ -4218,21 +4222,21 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>37</v>
@@ -4241,19 +4245,19 @@
         <v>37</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
@@ -4267,7 +4271,7 @@
         <v>37</v>
       </c>
       <c r="T27" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U27" t="s" s="2">
         <v>37</v>
@@ -4303,22 +4307,22 @@
         <v>37</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>37</v>
@@ -4326,39 +4330,39 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H28" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I28" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -4385,13 +4389,13 @@
         <v>37</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="Z28" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AA28" t="s" s="2">
         <v>37</v>
@@ -4409,22 +4413,22 @@
         <v>37</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH28" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI28" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>37</v>
@@ -4432,39 +4436,39 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H29" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I29" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -4479,7 +4483,7 @@
         <v>37</v>
       </c>
       <c r="T29" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="U29" t="s" s="2">
         <v>37</v>
@@ -4515,22 +4519,22 @@
         <v>37</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI29" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>37</v>
@@ -4538,10 +4542,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4552,7 +4556,7 @@
         <v>38</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>37</v>
@@ -4561,19 +4565,19 @@
         <v>37</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -4623,22 +4627,22 @@
         <v>37</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI30" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>37</v>
@@ -4646,10 +4650,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -4660,7 +4664,7 @@
         <v>38</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H31" t="s" s="2">
         <v>37</v>
@@ -4669,20 +4673,20 @@
         <v>37</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>37</v>
@@ -4695,7 +4699,7 @@
         <v>37</v>
       </c>
       <c r="T31" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="U31" t="s" s="2">
         <v>37</v>
@@ -4731,22 +4735,22 @@
         <v>37</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH31" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI31" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>37</v>
@@ -4754,10 +4758,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -4768,7 +4772,7 @@
         <v>38</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>37</v>
@@ -4777,20 +4781,20 @@
         <v>37</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="P32" t="s" s="2">
         <v>37</v>
@@ -4815,13 +4819,13 @@
         <v>37</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Z32" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AA32" t="s" s="2">
         <v>37</v>
@@ -4839,33 +4843,33 @@
         <v>37</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH32" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI32" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -4876,7 +4880,7 @@
         <v>38</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>37</v>
@@ -4888,17 +4892,17 @@
         <v>37</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="P33" t="s" s="2">
         <v>37</v>
@@ -4947,22 +4951,22 @@
         <v>37</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AL33" t="s" s="2">
         <v>37</v>
@@ -4970,10 +4974,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -4984,7 +4988,7 @@
         <v>38</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>37</v>
@@ -4996,13 +5000,13 @@
         <v>37</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -5053,13 +5057,13 @@
         <v>37</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>37</v>
@@ -5068,7 +5072,7 @@
         <v>37</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AL34" t="s" s="2">
         <v>37</v>
@@ -5076,14 +5080,14 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -5102,16 +5106,16 @@
         <v>37</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -5161,7 +5165,7 @@
         <v>37</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>38</v>
@@ -5173,10 +5177,10 @@
         <v>37</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>37</v>
@@ -5184,14 +5188,14 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
@@ -5204,25 +5208,25 @@
         <v>37</v>
       </c>
       <c r="I36" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O36" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="P36" t="s" s="2">
         <v>37</v>
@@ -5271,7 +5275,7 @@
         <v>37</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>38</v>
@@ -5283,10 +5287,10 @@
         <v>37</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>37</v>
@@ -5294,10 +5298,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5305,10 +5309,10 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H37" t="s" s="2">
         <v>37</v>
@@ -5320,13 +5324,13 @@
         <v>37</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -5377,22 +5381,22 @@
         <v>37</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AL37" t="s" s="2">
         <v>37</v>
@@ -5400,10 +5404,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -5411,10 +5415,10 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>37</v>
@@ -5426,13 +5430,13 @@
         <v>37</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -5483,22 +5487,22 @@
         <v>37</v>
       </c>
       <c r="AF38" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="AG38" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH38" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AI38" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AJ38" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="AK38" t="s" s="2">
         <v>279</v>
-      </c>
-      <c r="AG38" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH38" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI38" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AJ38" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="AK38" t="s" s="2">
-        <v>278</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>37</v>
@@ -5506,10 +5510,10 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -5520,7 +5524,7 @@
         <v>38</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>37</v>
@@ -5532,13 +5536,13 @@
         <v>37</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -5589,22 +5593,22 @@
         <v>37</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>37</v>
@@ -5612,10 +5616,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -5626,31 +5630,31 @@
         <v>38</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I40" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O40" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="P40" t="s" s="2">
         <v>37</v>
@@ -5699,22 +5703,22 @@
         <v>37</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>37</v>
@@ -5722,10 +5726,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -5736,7 +5740,7 @@
         <v>38</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>37</v>
@@ -5748,17 +5752,17 @@
         <v>37</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="P41" t="s" s="2">
         <v>37</v>
@@ -5807,22 +5811,22 @@
         <v>37</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH41" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI41" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>37</v>
@@ -5830,10 +5834,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -5856,16 +5860,16 @@
         <v>37</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
@@ -5915,7 +5919,7 @@
         <v>37</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>38</v>
@@ -5927,10 +5931,10 @@
         <v>37</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>37</v>
@@ -5938,10 +5942,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -5952,7 +5956,7 @@
         <v>38</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>37</v>
@@ -5964,13 +5968,13 @@
         <v>37</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -6021,13 +6025,13 @@
         <v>37</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH43" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI43" t="s" s="2">
         <v>37</v>
@@ -6036,7 +6040,7 @@
         <v>37</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>37</v>
@@ -6044,14 +6048,14 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s" s="2">
@@ -6070,16 +6074,16 @@
         <v>37</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
@@ -6129,7 +6133,7 @@
         <v>37</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>38</v>
@@ -6141,10 +6145,10 @@
         <v>37</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>37</v>
@@ -6152,14 +6156,14 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
@@ -6172,25 +6176,25 @@
         <v>37</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O45" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="P45" t="s" s="2">
         <v>37</v>
@@ -6239,7 +6243,7 @@
         <v>37</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>38</v>
@@ -6251,10 +6255,10 @@
         <v>37</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>37</v>
@@ -6262,10 +6266,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6288,13 +6292,13 @@
         <v>37</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -6321,13 +6325,13 @@
         <v>37</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="Z46" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AA46" t="s" s="2">
         <v>37</v>
@@ -6345,7 +6349,7 @@
         <v>37</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>38</v>
@@ -6357,10 +6361,10 @@
         <v>37</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AL46" t="s" s="2">
         <v>37</v>
@@ -6368,10 +6372,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -6382,7 +6386,7 @@
         <v>38</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H47" t="s" s="2">
         <v>37</v>
@@ -6394,13 +6398,13 @@
         <v>37</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -6451,22 +6455,22 @@
         <v>37</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI47" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>37</v>
@@ -6474,10 +6478,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -6488,7 +6492,7 @@
         <v>38</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>37</v>
@@ -6500,13 +6504,13 @@
         <v>37</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -6557,22 +6561,22 @@
         <v>37</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>37</v>
@@ -6580,10 +6584,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -6594,7 +6598,7 @@
         <v>38</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H49" t="s" s="2">
         <v>37</v>
@@ -6606,13 +6610,13 @@
         <v>37</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -6663,22 +6667,22 @@
         <v>37</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>37</v>
@@ -6686,10 +6690,10 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -6700,7 +6704,7 @@
         <v>38</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H50" t="s" s="2">
         <v>37</v>
@@ -6712,13 +6716,13 @@
         <v>37</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -6769,22 +6773,22 @@
         <v>37</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH50" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AI50" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>37</v>
@@ -6792,10 +6796,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -6818,17 +6822,17 @@
         <v>37</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="P51" t="s" s="2">
         <v>37</v>
@@ -6877,7 +6881,7 @@
         <v>37</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>38</v>
@@ -6889,10 +6893,10 @@
         <v>37</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>37</v>

</xml_diff>